<commit_message>
Started tidying code, making this Cmake compatible
</commit_message>
<xml_diff>
--- a/Pathfinder ANN/Genetic Algorithms/ANN Tests/Phase 0 (fail)/Attempt 3 (fail)/Difchecker (Attempt 3, Between Cycle 1 and Cycle 10000000).xlsx
+++ b/Pathfinder ANN/Genetic Algorithms/ANN Tests/Phase 0 (fail)/Attempt 3 (fail)/Difchecker (Attempt 3, Between Cycle 1 and Cycle 10000000).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Skoll\OneDrive - Bournemouth University\Work\Year 3\Final Year Project\Analytics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Skoll\OneDrive - Bournemouth University\Work\Year 3\Final Year Project\Pathfinder-AI\Pathfinder ANN\Genetic Algorithms\ANN Tests\Phase 0 (fail)\Attempt 3 (fail)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{567ED951-D7E1-4E00-A385-6A21302BF7BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA0250C1-9A70-43FD-8706-2C661CF89FD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4267,7 +4267,7 @@
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -4305,7 +4305,8 @@
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
+        <c:lblOffset val="1"/>
+        <c:tickLblSkip val="100"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
@@ -4361,7 +4362,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="557413608"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -5278,8 +5279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AYV1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB19" sqref="AB19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O41" sqref="O41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>